<commit_message>
repair docx & fix xlxs
</commit_message>
<xml_diff>
--- a/TA bab 1-4/learndata aimdata combined.xlsx
+++ b/TA bab 1-4/learndata aimdata combined.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tugas Akhir\TA Git\Tugas-Akhir\TA bab 1-4\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
@@ -15,8 +10,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -41,8 +36,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,18 +86,8 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="id-ID"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -111,7 +96,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -136,7 +121,6 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -144,33 +128,11 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -815,8 +777,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6CB5-4D48-93A9-C610D7DFD340}"/>
             </c:ext>
@@ -1466,8 +1427,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6CB5-4D48-93A9-C610D7DFD340}"/>
             </c:ext>
@@ -2117,31 +2077,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-6CB5-4D48-93A9-C610D7DFD340}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="2005999552"/>
-        <c:axId val="2006011200"/>
+        <c:dLbls/>
+        <c:marker val="1"/>
+        <c:axId val="97986048"/>
+        <c:axId val="97987968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2005999552"/>
+        <c:axId val="97986048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -2150,7 +2101,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -2170,7 +2121,6 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -2178,30 +2128,9 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2221,7 +2150,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2233,22 +2162,21 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2006011200"/>
+        <c:crossAx val="97987968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
+        <c:tickLblSkip val="10"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2006011200"/>
+        <c:axId val="97987968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2271,7 +2199,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -2291,7 +2219,6 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -2299,30 +2226,9 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2336,7 +2242,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2348,10 +2254,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2005999552"/>
+        <c:crossAx val="97986048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2366,7 +2272,6 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2379,7 +2284,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2391,13 +2296,12 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="id-ID"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2421,30 +2325,20 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="id-ID"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="id-ID"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2453,7 +2347,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2473,7 +2367,6 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2481,33 +2374,11 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -3152,8 +3023,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2D68-4496-8DB7-C3B508028991}"/>
             </c:ext>
@@ -3803,8 +3673,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2D68-4496-8DB7-C3B508028991}"/>
             </c:ext>
@@ -4454,31 +4323,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-2D68-4496-8DB7-C3B508028991}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="1974369792"/>
-        <c:axId val="1974363552"/>
+        <c:dLbls/>
+        <c:marker val="1"/>
+        <c:axId val="98699520"/>
+        <c:axId val="98713984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1974369792"/>
+        <c:axId val="98699520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -4487,7 +4347,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -4507,7 +4367,6 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -4515,30 +4374,9 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -4558,7 +4396,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4570,22 +4408,21 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1974363552"/>
+        <c:crossAx val="98713984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
+        <c:tickLblSkip val="10"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1974363552"/>
+        <c:axId val="98713984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -4608,7 +4445,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -4628,7 +4465,6 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -4636,30 +4472,9 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -4673,7 +4488,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4685,10 +4500,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1974369792"/>
+        <c:crossAx val="98699520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4703,7 +4518,6 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -4716,7 +4530,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -4728,13 +4542,12 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="id-ID"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4758,30 +4571,20 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="id-ID"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="id-ID"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -4790,7 +4593,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4815,7 +4618,6 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -4823,33 +4625,11 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -5494,8 +5274,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-71A2-4102-8BCB-E106B0723BE0}"/>
             </c:ext>
@@ -6145,8 +5924,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-71A2-4102-8BCB-E106B0723BE0}"/>
             </c:ext>
@@ -6796,31 +6574,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-71A2-4102-8BCB-E106B0723BE0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="1973563360"/>
-        <c:axId val="1973586656"/>
+        <c:dLbls/>
+        <c:marker val="1"/>
+        <c:axId val="98749440"/>
+        <c:axId val="98784384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1973563360"/>
+        <c:axId val="98749440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -6829,7 +6598,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -6854,7 +6623,6 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -6862,30 +6630,9 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -6905,7 +6652,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -6917,22 +6664,21 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1973586656"/>
+        <c:crossAx val="98784384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
+        <c:tickLblSkip val="10"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1973586656"/>
+        <c:axId val="98784384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -6955,7 +6701,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -6975,7 +6721,6 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -6983,30 +6728,9 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -7020,7 +6744,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -7032,10 +6756,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1973563360"/>
+        <c:crossAx val="98749440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7050,7 +6774,6 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -7063,7 +6786,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -7075,13 +6798,12 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="id-ID"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -7105,12 +6827,12 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="id-ID"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8922,7 +8644,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -8957,7 +8679,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -9134,23 +8856,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:O103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M13" workbookViewId="0">
-      <selection activeCell="AA40" sqref="AA40"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -9188,7 +8910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15">
       <c r="B4">
         <v>1</v>
       </c>
@@ -9226,7 +8948,7 @@
         <v>341.99999999999898</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15">
       <c r="B5">
         <v>2</v>
       </c>
@@ -9264,7 +8986,7 @@
         <v>630.04</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15">
       <c r="B6">
         <v>3</v>
       </c>
@@ -9302,7 +9024,7 @@
         <v>669.13999999999896</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15">
       <c r="B7">
         <v>4</v>
       </c>
@@ -9340,7 +9062,7 @@
         <v>675.86</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15">
       <c r="B8">
         <v>5</v>
       </c>
@@ -9378,7 +9100,7 @@
         <v>840.43</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15">
       <c r="B9">
         <v>6</v>
       </c>
@@ -9416,7 +9138,7 @@
         <v>324.51</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15">
       <c r="B10">
         <v>7</v>
       </c>
@@ -9454,7 +9176,7 @@
         <v>604.28999999999905</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15">
       <c r="B11">
         <v>8</v>
       </c>
@@ -9492,7 +9214,7 @@
         <v>354.55</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15">
       <c r="B12">
         <v>9</v>
       </c>
@@ -9530,7 +9252,7 @@
         <v>613.63</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15">
       <c r="B13">
         <v>10</v>
       </c>
@@ -9568,7 +9290,7 @@
         <v>709.28</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15">
       <c r="B14">
         <v>11</v>
       </c>
@@ -9606,7 +9328,7 @@
         <v>330.469999999999</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15">
       <c r="B15">
         <v>12</v>
       </c>
@@ -9644,7 +9366,7 @@
         <v>411.539999999999</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15">
       <c r="B16">
         <v>13</v>
       </c>
@@ -9682,7 +9404,7 @@
         <v>503.35999999999899</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15">
       <c r="B17">
         <v>14</v>
       </c>
@@ -9720,7 +9442,7 @@
         <v>563.70000000000005</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15">
       <c r="B18">
         <v>15</v>
       </c>
@@ -9758,7 +9480,7 @@
         <v>519.01999999999896</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15">
       <c r="B19">
         <v>16</v>
       </c>
@@ -9796,7 +9518,7 @@
         <v>375.3</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15">
       <c r="B20">
         <v>17</v>
       </c>
@@ -9834,7 +9556,7 @@
         <v>645.40999999999894</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15">
       <c r="B21">
         <v>18</v>
       </c>
@@ -9872,7 +9594,7 @@
         <v>455.64999999999901</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15">
       <c r="B22">
         <v>19</v>
       </c>
@@ -9910,7 +9632,7 @@
         <v>312.479999999999</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15">
       <c r="B23">
         <v>20</v>
       </c>
@@ -9948,7 +9670,7 @@
         <v>488.50999999999902</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15">
       <c r="B24">
         <v>21</v>
       </c>
@@ -9986,7 +9708,7 @@
         <v>814.47</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15">
       <c r="B25">
         <v>22</v>
       </c>
@@ -10024,7 +9746,7 @@
         <v>406.41999999999899</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:15">
       <c r="B26">
         <v>23</v>
       </c>
@@ -10062,7 +9784,7 @@
         <v>441.77999999999901</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:15">
       <c r="B27">
         <v>24</v>
       </c>
@@ -10100,7 +9822,7 @@
         <v>373.56999999999903</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:15">
       <c r="B28">
         <v>25</v>
       </c>
@@ -10138,7 +9860,7 @@
         <v>337.46</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:15">
       <c r="B29">
         <v>26</v>
       </c>
@@ -10176,7 +9898,7 @@
         <v>400.34</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:15">
       <c r="B30">
         <v>27</v>
       </c>
@@ -10214,7 +9936,7 @@
         <v>591.27</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:15">
       <c r="B31">
         <v>28</v>
       </c>
@@ -10252,7 +9974,7 @@
         <v>778.15999999999894</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:15">
       <c r="B32">
         <v>29</v>
       </c>
@@ -10290,7 +10012,7 @@
         <v>496.659999999999</v>
       </c>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:15">
       <c r="B33">
         <v>30</v>
       </c>
@@ -10328,7 +10050,7 @@
         <v>524.37</v>
       </c>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:15">
       <c r="B34">
         <v>31</v>
       </c>
@@ -10366,7 +10088,7 @@
         <v>522.53</v>
       </c>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:15">
       <c r="B35">
         <v>32</v>
       </c>
@@ -10404,7 +10126,7 @@
         <v>611.52</v>
       </c>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:15">
       <c r="B36">
         <v>33</v>
       </c>
@@ -10442,7 +10164,7 @@
         <v>740.07</v>
       </c>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:15">
       <c r="B37">
         <v>34</v>
       </c>
@@ -10480,7 +10202,7 @@
         <v>680.85</v>
       </c>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:15">
       <c r="B38">
         <v>35</v>
       </c>
@@ -10518,7 +10240,7 @@
         <v>541.60999999999899</v>
       </c>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:15">
       <c r="B39">
         <v>36</v>
       </c>
@@ -10556,7 +10278,7 @@
         <v>364.41</v>
       </c>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:15">
       <c r="B40">
         <v>37</v>
       </c>
@@ -10594,7 +10316,7 @@
         <v>497.48999999999899</v>
       </c>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:15">
       <c r="B41">
         <v>38</v>
       </c>
@@ -10632,7 +10354,7 @@
         <v>351.42999999999898</v>
       </c>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:15">
       <c r="B42">
         <v>39</v>
       </c>
@@ -10670,7 +10392,7 @@
         <v>157.60999999999899</v>
       </c>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:15">
       <c r="B43">
         <v>40</v>
       </c>
@@ -10708,7 +10430,7 @@
         <v>571.56999999999903</v>
       </c>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:15">
       <c r="B44">
         <v>41</v>
       </c>
@@ -10746,7 +10468,7 @@
         <v>656.03</v>
       </c>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:15">
       <c r="B45">
         <v>42</v>
       </c>
@@ -10784,7 +10506,7 @@
         <v>761.41</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:15">
       <c r="B46">
         <v>43</v>
       </c>
@@ -10822,7 +10544,7 @@
         <v>535.59</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:15">
       <c r="B47">
         <v>44</v>
       </c>
@@ -10860,7 +10582,7 @@
         <v>672.71</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:15">
       <c r="B48">
         <v>45</v>
       </c>
@@ -10898,7 +10620,7 @@
         <v>487.539999999999</v>
       </c>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:15">
       <c r="B49">
         <v>46</v>
       </c>
@@ -10936,7 +10658,7 @@
         <v>556.53</v>
       </c>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:15">
       <c r="B50">
         <v>47</v>
       </c>
@@ -10974,7 +10696,7 @@
         <v>528.77</v>
       </c>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:15">
       <c r="B51">
         <v>48</v>
       </c>
@@ -11012,7 +10734,7 @@
         <v>630.37</v>
       </c>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:15">
       <c r="B52">
         <v>49</v>
       </c>
@@ -11050,7 +10772,7 @@
         <v>536.979999999999</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:15">
       <c r="B53">
         <v>50</v>
       </c>
@@ -11088,7 +10810,7 @@
         <v>663.06999999999903</v>
       </c>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:15">
       <c r="B54">
         <v>51</v>
       </c>
@@ -11126,7 +10848,7 @@
         <v>676.30999999999904</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:15">
       <c r="B55">
         <v>52</v>
       </c>
@@ -11164,7 +10886,7 @@
         <v>738.11</v>
       </c>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:15">
       <c r="B56">
         <v>53</v>
       </c>
@@ -11202,7 +10924,7 @@
         <v>391.84</v>
       </c>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:15">
       <c r="B57">
         <v>54</v>
       </c>
@@ -11240,7 +10962,7 @@
         <v>851.43</v>
       </c>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:15">
       <c r="B58">
         <v>55</v>
       </c>
@@ -11278,7 +11000,7 @@
         <v>701.61999999999898</v>
       </c>
     </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:15">
       <c r="B59">
         <v>56</v>
       </c>
@@ -11316,7 +11038,7 @@
         <v>870.67</v>
       </c>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:15">
       <c r="B60">
         <v>57</v>
       </c>
@@ -11354,7 +11076,7 @@
         <v>692.29</v>
       </c>
     </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:15">
       <c r="B61">
         <v>58</v>
       </c>
@@ -11392,7 +11114,7 @@
         <v>652.60999999999899</v>
       </c>
     </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:15">
       <c r="B62">
         <v>59</v>
       </c>
@@ -11430,7 +11152,7 @@
         <v>633.63</v>
       </c>
     </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:15">
       <c r="B63">
         <v>60</v>
       </c>
@@ -11468,7 +11190,7 @@
         <v>595.33000000000004</v>
       </c>
     </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:15">
       <c r="B64">
         <v>61</v>
       </c>
@@ -11506,7 +11228,7 @@
         <v>975.04</v>
       </c>
     </row>
-    <row r="65" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:15">
       <c r="B65">
         <v>62</v>
       </c>
@@ -11544,7 +11266,7 @@
         <v>602.25999999999897</v>
       </c>
     </row>
-    <row r="66" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:15">
       <c r="B66">
         <v>63</v>
       </c>
@@ -11582,7 +11304,7 @@
         <v>951.27999999999895</v>
       </c>
     </row>
-    <row r="67" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:15">
       <c r="B67">
         <v>64</v>
       </c>
@@ -11620,7 +11342,7 @@
         <v>646.65999999999894</v>
       </c>
     </row>
-    <row r="68" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:15">
       <c r="B68">
         <v>65</v>
       </c>
@@ -11658,7 +11380,7 @@
         <v>750.16</v>
       </c>
     </row>
-    <row r="69" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:15">
       <c r="B69">
         <v>66</v>
       </c>
@@ -11696,7 +11418,7 @@
         <v>882.13</v>
       </c>
     </row>
-    <row r="70" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:15">
       <c r="B70">
         <v>67</v>
       </c>
@@ -11734,7 +11456,7 @@
         <v>478.53</v>
       </c>
     </row>
-    <row r="71" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:15">
       <c r="B71">
         <v>68</v>
       </c>
@@ -11772,7 +11494,7 @@
         <v>570.69000000000005</v>
       </c>
     </row>
-    <row r="72" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:15">
       <c r="B72">
         <v>69</v>
       </c>
@@ -11810,7 +11532,7 @@
         <v>345.11999999999898</v>
       </c>
     </row>
-    <row r="73" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:15">
       <c r="B73">
         <v>70</v>
       </c>
@@ -11848,7 +11570,7 @@
         <v>531.32999999999902</v>
       </c>
     </row>
-    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:15">
       <c r="B74">
         <v>71</v>
       </c>
@@ -11886,7 +11608,7 @@
         <v>564.25999999999897</v>
       </c>
     </row>
-    <row r="75" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:15">
       <c r="B75">
         <v>72</v>
       </c>
@@ -11924,7 +11646,7 @@
         <v>811.36999999999898</v>
       </c>
     </row>
-    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:15">
       <c r="B76">
         <v>73</v>
       </c>
@@ -11962,7 +11684,7 @@
         <v>619.87</v>
       </c>
     </row>
-    <row r="77" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:15">
       <c r="B77">
         <v>74</v>
       </c>
@@ -12000,7 +11722,7 @@
         <v>284.32999999999902</v>
       </c>
     </row>
-    <row r="78" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:15">
       <c r="B78">
         <v>75</v>
       </c>
@@ -12038,7 +11760,7 @@
         <v>569.93999999999903</v>
       </c>
     </row>
-    <row r="79" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:15">
       <c r="B79">
         <v>76</v>
       </c>
@@ -12076,7 +11798,7 @@
         <v>643.83999999999901</v>
       </c>
     </row>
-    <row r="80" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:15">
       <c r="B80">
         <v>77</v>
       </c>
@@ -12114,7 +11836,7 @@
         <v>633.36</v>
       </c>
     </row>
-    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:15">
       <c r="B81">
         <v>78</v>
       </c>
@@ -12152,7 +11874,7 @@
         <v>260.02</v>
       </c>
     </row>
-    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:15">
       <c r="B82">
         <v>79</v>
       </c>
@@ -12190,7 +11912,7 @@
         <v>828.15</v>
       </c>
     </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:15">
       <c r="B83">
         <v>80</v>
       </c>
@@ -12228,7 +11950,7 @@
         <v>662.52</v>
       </c>
     </row>
-    <row r="84" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:15">
       <c r="B84">
         <v>81</v>
       </c>
@@ -12266,7 +11988,7 @@
         <v>533.46</v>
       </c>
     </row>
-    <row r="85" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:15">
       <c r="B85">
         <v>82</v>
       </c>
@@ -12304,7 +12026,7 @@
         <v>805.18999999999903</v>
       </c>
     </row>
-    <row r="86" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:15">
       <c r="B86">
         <v>83</v>
       </c>
@@ -12342,7 +12064,7 @@
         <v>629.61999999999898</v>
       </c>
     </row>
-    <row r="87" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:15">
       <c r="B87">
         <v>84</v>
       </c>
@@ -12380,7 +12102,7 @@
         <v>330.76999999999902</v>
       </c>
     </row>
-    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:15">
       <c r="B88">
         <v>85</v>
       </c>
@@ -12418,7 +12140,7 @@
         <v>668.85999999999899</v>
       </c>
     </row>
-    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:15">
       <c r="B89">
         <v>86</v>
       </c>
@@ -12456,7 +12178,7 @@
         <v>766.04</v>
       </c>
     </row>
-    <row r="90" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:15">
       <c r="B90">
         <v>87</v>
       </c>
@@ -12494,7 +12216,7 @@
         <v>440.77</v>
       </c>
     </row>
-    <row r="91" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:15">
       <c r="B91">
         <v>88</v>
       </c>
@@ -12532,7 +12254,7 @@
         <v>622.979999999999</v>
       </c>
     </row>
-    <row r="92" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:15">
       <c r="B92">
         <v>89</v>
       </c>
@@ -12570,7 +12292,7 @@
         <v>582.91999999999905</v>
       </c>
     </row>
-    <row r="93" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:15">
       <c r="B93">
         <v>90</v>
       </c>
@@ -12608,7 +12330,7 @@
         <v>343.88999999999902</v>
       </c>
     </row>
-    <row r="94" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:15">
       <c r="B94">
         <v>91</v>
       </c>
@@ -12646,7 +12368,7 @@
         <v>278.79000000000002</v>
       </c>
     </row>
-    <row r="95" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:15">
       <c r="B95">
         <v>92</v>
       </c>
@@ -12684,7 +12406,7 @@
         <v>377.57</v>
       </c>
     </row>
-    <row r="96" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:15">
       <c r="B96">
         <v>93</v>
       </c>
@@ -12722,7 +12444,7 @@
         <v>419.65</v>
       </c>
     </row>
-    <row r="97" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:15">
       <c r="B97">
         <v>94</v>
       </c>
@@ -12760,7 +12482,7 @@
         <v>377.02999999999901</v>
       </c>
     </row>
-    <row r="98" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:15">
       <c r="B98">
         <v>95</v>
       </c>
@@ -12798,7 +12520,7 @@
         <v>616.33999999999901</v>
       </c>
     </row>
-    <row r="99" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:15">
       <c r="B99">
         <v>96</v>
       </c>
@@ -12836,7 +12558,7 @@
         <v>415.02999999999901</v>
       </c>
     </row>
-    <row r="100" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:15">
       <c r="B100">
         <v>97</v>
       </c>
@@ -12874,7 +12596,7 @@
         <v>552.52999999999895</v>
       </c>
     </row>
-    <row r="101" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:15">
       <c r="B101">
         <v>98</v>
       </c>
@@ -12912,7 +12634,7 @@
         <v>705.18999999999903</v>
       </c>
     </row>
-    <row r="102" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:15">
       <c r="B102">
         <v>99</v>
       </c>
@@ -12950,7 +12672,7 @@
         <v>502.63999999999902</v>
       </c>
     </row>
-    <row r="103" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:15">
       <c r="B103">
         <v>100</v>
       </c>

</xml_diff>